<commit_message>
fix: correct workspace sharing links
</commit_message>
<xml_diff>
--- a/ExcelSheets/SimpleBatteryCharging.xlsx
+++ b/ExcelSheets/SimpleBatteryCharging.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A60A80D-ABC6-4BE9-90BE-8B28DB35A3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4064A1D-98F5-4BA2-85F5-2518DD61A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -379,7 +379,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1155,13 +1155,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1186,6 +1179,7 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="18" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1205,6 +1199,12 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1597,7 +1597,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1651,12 +1651,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F82F9D3-D2C7-4C41-930E-2A93B4D9DAF4}" type="CELLRANGE">
+                    <a:fld id="{F68F7642-C749-4F32-B05C-A6235127205A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1684,12 +1684,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35B927AF-3089-49AE-AD59-442D3AE6BD94}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4A25A495-0908-4513-8F00-81B63CA3EBA4}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1718,12 +1718,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27EFCA26-D6B0-45FD-8BE4-BF2AC64D3E46}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{B64850D2-DA8C-4615-B912-4FF0F772DAF4}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1752,12 +1752,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E74300E8-8E0B-405C-95C5-460987FC1F9D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7CEB28D6-F36D-4356-90F7-9C11BF8BB021}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1786,12 +1786,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C373623C-FF17-4869-AA52-EA15F9BBDC08}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9ED9C8E1-07B6-4218-923C-8F6DD816172A}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1820,12 +1820,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB7361DA-5C82-4DD4-8D48-1441B9D13EAA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{398E75BB-5889-489F-8DEC-AFB02450FAC3}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1854,12 +1854,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E12013B-ABCF-417F-B8DA-31ED7B08E437}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{59ACE9C7-BEA6-458F-968C-AAA595553A90}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1888,12 +1888,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05D291CF-7811-4386-8C87-30FC1F55CC40}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{75F52580-EB60-49ED-B1E8-8DF31BB573F9}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1922,12 +1922,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6F6328E-D0DE-42D5-8611-7F3EDD0BE021}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D46A55DF-FB5C-4420-8EDC-D473C1907CC6}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1956,12 +1956,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBB15D4D-873C-485D-9603-568EA103B5B1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0D5656F6-E3DB-4659-AE99-DBFDB2F86A45}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1990,12 +1990,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02833AE2-21F8-476F-9FF7-5FB981A39B48}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{8E6EFFAA-D742-4946-80F0-1A990A350968}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2024,12 +2024,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA691464-CDCD-42D4-98CD-92487C4A04F1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{15FB13CE-DD63-42B8-B528-3FDB2B9F6FDF}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2058,12 +2058,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FCFC22C-19D4-4AD8-AF25-6F78B5754C19}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{27666DB1-569C-4F2B-862F-815795A03E81}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2092,12 +2092,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D8935FC-A51F-4588-8637-3E92325747E9}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{EB977E01-BF39-471D-B5ED-7A20D612D286}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2126,12 +2126,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3331BCE1-2533-4802-980E-63F4E7FDFB27}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{245F7D05-C48E-4338-A474-858440244293}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2160,12 +2160,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F41FE02-D5EE-4BC9-83CD-72578284FDD0}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{CD2DB2AB-9285-4BA2-97CB-051F1D729F4D}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2194,12 +2194,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63E4F32B-ED92-463A-9C1F-4121471D13D6}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{ED86ADD0-51D3-4E18-99D1-861F1CD39AFD}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2228,12 +2228,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75112A54-AFB0-477E-B98C-958B02A704BD}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{931FB98B-0540-4B6B-8EDA-72683CEC5408}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2262,12 +2262,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BCF1545-D202-4453-9552-C37645356ABF}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2583F514-57E4-496D-A945-24C96F22E22D}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2296,12 +2296,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{470A35B4-C69B-453B-A563-47B2989FDD28}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{56E71F4D-605F-4E88-B92C-BB76136452BF}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2330,12 +2330,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AE5E7E5-69F3-4B48-8445-7868AC57D10D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{007E4CC4-AC0E-4796-80E0-CE344422A2CF}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2364,12 +2364,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BB8DB90-7015-4616-966A-9F1FA520EBA9}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{6385402D-D420-45A6-B5EC-46D4CA4C8050}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2398,12 +2398,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D85A0AA0-7E28-48C1-80C6-6175CFC19E2B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0C242D57-95ED-4CF4-BD68-6FBDD8D12365}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2451,7 +2451,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-SE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2793,7 +2793,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2831,7 +2831,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1337863680"/>
@@ -2904,7 +2904,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2942,7 +2942,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1337868928"/>
@@ -2990,7 +2990,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-SE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3066,7 +3066,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3304,12 +3304,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C32A02DB-B6EF-4B19-B40E-220D853AD59E}" type="CELLRANGE">
+                    <a:fld id="{29DA302C-6006-435E-88AD-50790A66A972}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3337,12 +3337,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDC5D9CE-7A36-4055-AC4C-A0A7C2323EBE}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{3AB4B6A4-CC1A-4A79-BEC8-B13E68588831}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3371,12 +3371,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C299258F-09D6-4AD2-9EBB-0FE996A13FEC}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{FD9BDA3E-1183-40DF-9703-82D52CC8B277}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3405,12 +3405,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2704B4B1-BF9C-44AC-B165-6032A6C07832}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{8190353D-F681-469A-BB46-2C14AAF9AB80}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3439,12 +3439,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA436C01-FF05-4C0D-BCA2-DD78641DDDCA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{BA093B48-A810-41F2-88FA-07432B9BE322}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3473,12 +3473,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBC1B258-647C-44D3-9197-906E476DF8A2}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{3C15857B-8B25-4103-90C8-F0F783F3C8B4}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3507,12 +3507,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{730DFE19-4A4E-437E-8886-94210A2A75B8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{323DCC75-9F99-48D1-9F96-18AD2F0EB27E}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3541,12 +3541,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CA0C4B7-9638-4B9A-BE1F-10583A39E4DD}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{8CFA4009-7179-4DB3-ABDA-4427D7488D7A}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3575,12 +3575,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D4FC5F1-B8FA-444F-91E9-94D76C470732}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2921CC03-1145-48A1-AB5F-19008691207D}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3609,12 +3609,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7FA416A-F244-4EEA-8026-9E94B47DB7A8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{CE61A13D-449E-4B39-8383-328E6034D539}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3643,12 +3643,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A70ECFF-D09D-40E0-9C15-51924C96DDA8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D531DAF3-2508-4E47-A990-144ACBBC0C86}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3677,12 +3677,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A501CA88-0F43-4AFE-A75B-10F4383761D1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D281CB2A-52C9-419A-8CB1-C7ABB91A83DB}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3711,12 +3711,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F904AD59-747F-45F4-AD03-0ECDBC46FDD9}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2C0E0A7B-317A-4489-9D1B-A94F74D304C1}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3745,12 +3745,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B520698-7111-466A-996A-C4A26E07BFA9}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7E9D6517-160D-4FBF-B338-36BC66D0C82F}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3779,12 +3779,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A716F097-A067-4602-A0C5-1B5127F2865C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{02D60AED-9C6D-4788-9A33-48552F6BD2A4}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3813,12 +3813,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34F8AF88-552B-4941-9801-61E4D63D6946}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4C92E084-10DB-454E-B93C-44F2703993E2}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3847,12 +3847,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C9D9162-ED5B-4B4B-8712-3A21051D0371}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{43A647C2-A89A-42B1-85A5-CBC2F165AE85}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3881,12 +3881,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1814D299-9E88-4233-BA84-6573F6471A74}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{706160F1-BF25-4AF0-A4C4-46829F4B18D7}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3915,12 +3915,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED35B4D2-F77A-44FC-8D9B-8821F8AC4AD5}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0FB165A2-6135-46C2-883E-3413BCECBFCF}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3949,12 +3949,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E33FB5A-4E4A-437F-8965-3A35A2EFFF92}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{95D10F79-7D5C-4EA1-9B66-CBB911DF74EC}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3983,12 +3983,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C810C6C-6CC7-4D5F-B98D-E38D3ABA1B08}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{187BDCCF-C11A-4C6E-A822-D1E0C8CCA1D2}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4017,12 +4017,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D05694AD-045D-49A4-890B-8502EF9B3AC6}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F0BC7723-3E6B-4D76-8F2F-14193DA7B295}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4051,12 +4051,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82E73D53-78BE-445E-A102-08678487E361}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9C21F5DB-9DD6-4EF3-A9F3-5AA0F6002C10}" type="CELLRANGE">
+                      <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4085,7 +4085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4113,7 +4113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4141,7 +4141,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4169,7 +4169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4197,7 +4197,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4225,7 +4225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4253,7 +4253,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4281,7 +4281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4309,7 +4309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4337,7 +4337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4365,7 +4365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4393,7 +4393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4421,7 +4421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4449,7 +4449,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4477,7 +4477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4505,7 +4505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4533,7 +4533,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4561,7 +4561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4589,7 +4589,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4617,7 +4617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4645,7 +4645,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4673,7 +4673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4701,7 +4701,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4729,7 +4729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4757,7 +4757,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4785,7 +4785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4813,7 +4813,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4841,7 +4841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4869,7 +4869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4897,7 +4897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4925,7 +4925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4953,7 +4953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -4981,7 +4981,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SE"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -5028,7 +5028,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-SE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -5370,7 +5370,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5408,7 +5408,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1337863680"/>
@@ -5481,7 +5481,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5519,7 +5519,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1337868928"/>
@@ -5561,7 +5561,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-SE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5598,7 +5598,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-SE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7716,7 +7716,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
+                <a:rPr lang="en-SE" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -8194,10 +8194,10 @@
   <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
     <col min="2" max="2" width="86.140625" style="1" customWidth="1"/>
@@ -8206,85 +8206,85 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" s="2" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" s="2" customFormat="1">
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="2:3" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" s="2" customFormat="1">
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" s="2" customFormat="1">
       <c r="B6" s="1"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" s="2" customFormat="1">
       <c r="B7" s="1"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" s="2" customFormat="1">
       <c r="B8" s="1"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" s="2" customFormat="1">
       <c r="B9" s="1"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" s="2" customFormat="1">
       <c r="B10" s="1"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" s="2" customFormat="1">
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" s="2" customFormat="1">
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" s="2" customFormat="1">
       <c r="B13" s="1"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="2:3" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="C14" s="5"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="7"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="21"/>
       <c r="C21" s="72"/>
     </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1">
       <c r="B24" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="73" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" t="s">
         <v>94</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" s="1" t="s">
         <v>100</v>
       </c>
@@ -8300,27 +8300,27 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" s="75" t="s">
         <v>99</v>
       </c>
       <c r="C30" s="74"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" s="75"/>
       <c r="D31" s="76"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" s="73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10">
       <c r="B33" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" s="2" customFormat="1">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -8331,11 +8331,11 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" ht="20.25" customHeight="1"/>
+    <row r="47" spans="2:10">
       <c r="B47" s="9"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10">
       <c r="B48" s="9"/>
     </row>
   </sheetData>
@@ -8356,7 +8356,7 @@
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="10" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="10" bestFit="1" customWidth="1"/>
@@ -8364,7 +8364,7 @@
     <col min="4" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="20.25" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -8376,10 +8376,10 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="B5" s="13" t="s">
         <v>5</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" ht="20.25" customHeight="1" thickBot="1">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -8415,12 +8415,12 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="9" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="17.25" customHeight="1">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="17.25" customHeight="1">
       <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="B15" s="13" t="s">
         <v>20</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>6900</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="17.25" customHeight="1">
       <c r="B17" s="17" t="s">
         <v>21</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33">
       <c r="B18" t="s">
         <v>56</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33">
       <c r="B19" t="s">
         <v>57</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>27815.771767919399</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>4.8484848484848492E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33">
       <c r="B21" t="s">
         <v>59</v>
       </c>
@@ -9197,7 +9197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" ht="19.5" customHeight="1" thickBot="1">
       <c r="A23" s="16" t="s">
         <v>22</v>
       </c>
@@ -9234,8 +9234,8 @@
       <c r="AF23" s="16"/>
       <c r="AG23" s="16"/>
     </row>
-    <row r="24" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="17.25" customHeight="1"/>
+    <row r="25" spans="1:33" ht="17.25" customHeight="1">
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="17.25" customHeight="1">
       <c r="B26" s="10" t="s">
         <v>60</v>
       </c>
@@ -9366,7 +9366,7 @@
       <c r="AF26" s="24"/>
       <c r="AG26" s="25"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33">
       <c r="B27" s="10" t="s">
         <v>61</v>
       </c>
@@ -9401,12 +9401,12 @@
       <c r="AF27" s="23"/>
       <c r="AG27" s="22"/>
     </row>
-    <row r="29" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" ht="17.25" customHeight="1">
       <c r="B29" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33">
       <c r="B30" s="10" t="s">
         <v>25</v>
       </c>
@@ -9441,7 +9441,7 @@
       <c r="AF30"/>
       <c r="AG30"/>
     </row>
-    <row r="31" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" ht="17.25" customHeight="1">
       <c r="B31" s="10" t="s">
         <v>26</v>
       </c>
@@ -9476,7 +9476,7 @@
       <c r="AF31"/>
       <c r="AG31"/>
     </row>
-    <row r="32" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="17.25" customHeight="1">
       <c r="B32" s="10" t="s">
         <v>27</v>
       </c>
@@ -9511,7 +9511,7 @@
       <c r="AF32"/>
       <c r="AG32"/>
     </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:33">
       <c r="B33" s="10" t="s">
         <v>28</v>
       </c>
@@ -9546,7 +9546,7 @@
       <c r="AF33"/>
       <c r="AG33"/>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:33">
       <c r="B34" s="10" t="s">
         <v>29</v>
       </c>
@@ -9581,7 +9581,7 @@
       <c r="AF34"/>
       <c r="AG34"/>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:33">
       <c r="B35" s="10" t="s">
         <v>30</v>
       </c>
@@ -9632,7 +9632,7 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -9645,7 +9645,7 @@
     <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="str" cm="1">
         <f t="array" ref="A1:K32">TRANSPOSE(ModelonExperiment!B17:AG27)</f>
         <v>Indata</v>
@@ -9681,7 +9681,7 @@
         <v>battery.summary.e_loss</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9716,7 +9716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="str">
         <v>Case 1</v>
       </c>
@@ -9751,7 +9751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="str">
         <v>Case 2</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="str">
         <v>Case 3</v>
       </c>
@@ -9821,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="str">
         <v>Case 4</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="str">
         <v>Case 5</v>
       </c>
@@ -9891,7 +9891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="str">
         <v>Case 6</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="str">
         <v>Case 7</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" t="str">
         <v>Case 8</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" t="str">
         <v>Case 9</v>
       </c>
@@ -10031,7 +10031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" t="str">
         <v>Case 10</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" t="str">
         <v>Case 11</v>
       </c>
@@ -10101,7 +10101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" t="str">
         <v>Case 12</v>
       </c>
@@ -10136,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" t="str">
         <v>Case 13</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" t="str">
         <v>Case 14</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" t="str">
         <v>Case 15</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" t="str">
         <v>Case 16</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" t="str">
         <v>Case 17</v>
       </c>
@@ -10311,7 +10311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" t="str">
         <v>Case 18</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" t="str">
         <v>Case 19</v>
       </c>
@@ -10381,7 +10381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" t="str">
         <v>Case 20</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" t="str">
         <v>Case 21</v>
       </c>
@@ -10451,7 +10451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="str">
         <v>Case 22</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" t="str">
         <v>Case 23</v>
       </c>
@@ -10521,7 +10521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" t="str">
         <v>Case 24</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" t="str">
         <v>Case 25</v>
       </c>
@@ -10591,7 +10591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" t="str">
         <v>Case 26</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" t="str">
         <v>Case 27</v>
       </c>
@@ -10661,7 +10661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" t="str">
         <v>Case 28</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" t="str">
         <v>Case 29</v>
       </c>
@@ -10731,7 +10731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" t="str">
         <v>Case 30</v>
       </c>
@@ -10780,7 +10780,7 @@
       <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="27" bestFit="1" customWidth="1"/>
@@ -10803,21 +10803,21 @@
     <col min="35" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:25" ht="52.5" customHeight="1">
+      <c r="A1" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
@@ -10832,7 +10832,7 @@
       <c r="X1" s="26"/>
       <c r="Y1" s="26"/>
     </row>
-    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="15" customHeight="1">
       <c r="A2" s="28"/>
       <c r="B2"/>
       <c r="C2" s="29"/>
@@ -10851,12 +10851,12 @@
       <c r="U2" s="29"/>
       <c r="V2" s="29"/>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+    <row r="3" spans="1:25" ht="15" customHeight="1">
+      <c r="A3" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
@@ -10867,14 +10867,14 @@
       <c r="U3" s="29"/>
       <c r="V3" s="29"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="15" customHeight="1">
       <c r="A4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="77"/>
+      <c r="C4" s="85"/>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
@@ -10887,14 +10887,14 @@
       <c r="U4" s="29"/>
       <c r="V4" s="29"/>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="85"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
@@ -10907,14 +10907,14 @@
       <c r="U5" s="29"/>
       <c r="V5" s="29"/>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="15" customHeight="1">
       <c r="A6" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="77"/>
+      <c r="C6" s="85"/>
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
@@ -10927,14 +10927,14 @@
       <c r="U6" s="29"/>
       <c r="V6" s="29"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="15" customHeight="1">
       <c r="A7" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="77"/>
+      <c r="C7" s="85"/>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -10947,14 +10947,14 @@
       <c r="U7" s="29"/>
       <c r="V7" s="29"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="15" customHeight="1">
       <c r="A8" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="85"/>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
@@ -10967,16 +10967,16 @@
       <c r="U8" s="29"/>
       <c r="V8" s="29"/>
     </row>
-    <row r="9" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="C9" s="29"/>
       <c r="D9" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="88" t="str">
+      <c r="E9" s="86" t="str">
         <f>_xlfn.CONCAT(B5," vs. ",B4)</f>
         <v>Cell Internal Resitance (Ω) vs. Cell Nominal Capacity (Ah)</v>
       </c>
-      <c r="F9" s="88"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="29"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
@@ -10989,16 +10989,16 @@
       <c r="U9" s="29"/>
       <c r="V9" s="29"/>
     </row>
-    <row r="10" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="C10" s="29"/>
       <c r="D10" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="89" t="str">
+      <c r="E10" s="87" t="str">
         <f>_xlfn.CONCAT(B8)</f>
         <v>Cell Max Charge Current (A)</v>
       </c>
-      <c r="F10" s="89"/>
+      <c r="F10" s="87"/>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
@@ -11011,7 +11011,7 @@
       <c r="U10" s="29"/>
       <c r="V10" s="29"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="15" customHeight="1">
       <c r="A11" s="28"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
@@ -11030,12 +11030,12 @@
       <c r="U11" s="29"/>
       <c r="V11" s="29"/>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90" t="s">
+    <row r="12" spans="1:25" ht="15" customHeight="1">
+      <c r="A12" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -11051,7 +11051,7 @@
       <c r="U12" s="29"/>
       <c r="V12" s="29"/>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="15" customHeight="1">
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -11070,7 +11070,7 @@
       <c r="U13" s="29"/>
       <c r="V13" s="29"/>
     </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="15" customHeight="1">
       <c r="A14" s="29"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -11089,7 +11089,7 @@
       <c r="U14" s="29"/>
       <c r="V14" s="29"/>
     </row>
-    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="15" customHeight="1">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -11108,7 +11108,7 @@
       <c r="U15" s="29"/>
       <c r="V15" s="29"/>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="15" customHeight="1">
       <c r="A16" s="29"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -11127,7 +11127,7 @@
       <c r="U16" s="29"/>
       <c r="V16" s="29"/>
     </row>
-    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="15" customHeight="1">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -11146,7 +11146,7 @@
       <c r="U17" s="29"/>
       <c r="V17" s="29"/>
     </row>
-    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" ht="15" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -11165,7 +11165,7 @@
       <c r="U18" s="29"/>
       <c r="V18" s="29"/>
     </row>
-    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="15" customHeight="1">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -11184,7 +11184,7 @@
       <c r="U19" s="29"/>
       <c r="V19" s="29"/>
     </row>
-    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" ht="15" customHeight="1">
       <c r="A20" s="29"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -11203,7 +11203,7 @@
       <c r="U20" s="29"/>
       <c r="V20" s="29"/>
     </row>
-    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="15" customHeight="1">
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -11222,7 +11222,7 @@
       <c r="U21" s="29"/>
       <c r="V21" s="29"/>
     </row>
-    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="15" customHeight="1">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -11241,7 +11241,7 @@
       <c r="U22" s="29"/>
       <c r="V22" s="29"/>
     </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="15" customHeight="1">
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -11260,7 +11260,7 @@
       <c r="U23" s="29"/>
       <c r="V23" s="29"/>
     </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="15" customHeight="1">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -11279,7 +11279,7 @@
       <c r="U24" s="29"/>
       <c r="V24" s="29"/>
     </row>
-    <row r="25" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="15" customHeight="1">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -11298,7 +11298,7 @@
       <c r="U25" s="29"/>
       <c r="V25" s="29"/>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="15" customHeight="1">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
@@ -11325,35 +11325,35 @@
       <c r="X26" s="29"/>
       <c r="Y26" s="29"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" s="91" t="s">
+    <row r="27" spans="1:25" ht="15">
+      <c r="A27" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="92"/>
-      <c r="C27" s="93" t="s">
+      <c r="B27" s="90"/>
+      <c r="C27" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="80" t="s">
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="81"/>
-      <c r="I27" s="82" t="s">
+      <c r="H27" s="78"/>
+      <c r="I27" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="83"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="85" t="s">
+      <c r="J27" s="80"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="M27" s="86"/>
-      <c r="N27" s="86"/>
-      <c r="O27" s="86"/>
-      <c r="P27" s="87"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M27" s="83"/>
+      <c r="N27" s="83"/>
+      <c r="O27" s="83"/>
+      <c r="P27" s="84"/>
+    </row>
+    <row r="28" spans="1:25" ht="15">
       <c r="A28" s="33" t="s">
         <v>29</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25">
       <c r="A29" s="45"/>
       <c r="B29" s="46">
         <v>1</v>
@@ -11465,7 +11465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25">
       <c r="A30" s="57"/>
       <c r="B30" s="58">
         <v>2</v>
@@ -11527,7 +11527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" hidden="1">
       <c r="A31" s="57"/>
       <c r="B31" s="58">
         <v>3</v>
@@ -11589,7 +11589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" hidden="1">
       <c r="A32" s="57"/>
       <c r="B32" s="58">
         <v>4</v>
@@ -11651,7 +11651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16">
       <c r="A33" s="57"/>
       <c r="B33" s="58">
         <v>5</v>
@@ -11713,7 +11713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16">
       <c r="A34" s="57"/>
       <c r="B34" s="58">
         <v>6</v>
@@ -11775,7 +11775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" hidden="1">
       <c r="A35" s="57"/>
       <c r="B35" s="58">
         <v>7</v>
@@ -11837,7 +11837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16">
       <c r="A36" s="57"/>
       <c r="B36" s="58">
         <v>8</v>
@@ -11899,7 +11899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" hidden="1">
       <c r="A37" s="57"/>
       <c r="B37" s="58">
         <v>9</v>
@@ -11961,7 +11961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16">
       <c r="A38" s="57"/>
       <c r="B38" s="58">
         <v>10</v>
@@ -12023,7 +12023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16">
       <c r="A39" s="57"/>
       <c r="B39" s="58">
         <v>11</v>
@@ -12085,7 +12085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16">
       <c r="A40" s="57"/>
       <c r="B40" s="58">
         <v>12</v>
@@ -12147,7 +12147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16">
       <c r="A41" s="57"/>
       <c r="B41" s="58">
         <v>13</v>
@@ -12209,7 +12209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" hidden="1">
       <c r="A42" s="57"/>
       <c r="B42" s="58">
         <v>14</v>
@@ -12271,7 +12271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16">
       <c r="A43" s="57"/>
       <c r="B43" s="58">
         <v>15</v>
@@ -12333,7 +12333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16">
       <c r="A44" s="57"/>
       <c r="B44" s="58">
         <v>16</v>
@@ -12395,7 +12395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16">
       <c r="A45" s="57"/>
       <c r="B45" s="58">
         <v>17</v>
@@ -12457,7 +12457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16">
       <c r="A46" s="57"/>
       <c r="B46" s="58">
         <v>18</v>
@@ -12519,7 +12519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16">
       <c r="A47" s="57"/>
       <c r="B47" s="58">
         <v>19</v>
@@ -12581,7 +12581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16">
       <c r="A48" s="57"/>
       <c r="B48" s="58">
         <v>20</v>
@@ -12643,7 +12643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16">
       <c r="A49" s="57"/>
       <c r="B49" s="58">
         <v>21</v>
@@ -12705,7 +12705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16">
       <c r="A50" s="57"/>
       <c r="B50" s="58">
         <v>22</v>
@@ -12767,7 +12767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16">
       <c r="A51" s="57"/>
       <c r="B51" s="58">
         <v>23</v>
@@ -12829,7 +12829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16">
       <c r="A52" s="57"/>
       <c r="B52" s="58">
         <v>24</v>
@@ -12891,7 +12891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16">
       <c r="A53" s="57"/>
       <c r="B53" s="58">
         <v>25</v>
@@ -12953,7 +12953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16">
       <c r="A54" s="57"/>
       <c r="B54" s="58">
         <v>26</v>
@@ -13015,7 +13015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16">
       <c r="A55" s="57"/>
       <c r="B55" s="58">
         <v>27</v>
@@ -13077,7 +13077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16">
       <c r="A56" s="57"/>
       <c r="B56" s="58">
         <v>28</v>
@@ -13139,7 +13139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" hidden="1">
       <c r="A57" s="57"/>
       <c r="B57" s="58">
         <v>29</v>
@@ -13201,7 +13201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" hidden="1">
       <c r="A58" s="57"/>
       <c r="B58" s="58">
         <v>30</v>
@@ -13269,6 +13269,12 @@
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="15">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="L27:P27"/>
@@ -13278,12 +13284,6 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:F27"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5 B8" xr:uid="{A7852E70-5BEE-4D66-A649-520BB2C90F33}">

</xml_diff>

<commit_message>
fix: removing open in impact link
</commit_message>
<xml_diff>
--- a/ExcelSheets/SimpleBatteryCharging.xlsx
+++ b/ExcelSheets/SimpleBatteryCharging.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4064A1D-98F5-4BA2-85F5-2518DD61A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A9D02A-2119-4CB1-AF63-1A193B5C495D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
   <si>
     <t>Introduction</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>Title Histogram:</t>
-  </si>
-  <si>
-    <t>Open in Modelon Impact</t>
   </si>
   <si>
     <t>Experiment</t>
@@ -1155,6 +1152,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1179,7 +1183,6 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="18" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1199,12 +1202,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1651,7 +1648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F68F7642-C749-4F32-B05C-A6235127205A}" type="CELLRANGE">
+                    <a:fld id="{7C2EEAB0-36AD-445F-8456-4A5CF7DE1C30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1684,7 +1681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A25A495-0908-4513-8F00-81B63CA3EBA4}" type="CELLRANGE">
+                    <a:fld id="{043FDCDD-DA28-4637-A4F0-3F80BE19E781}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1718,7 +1715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B64850D2-DA8C-4615-B912-4FF0F772DAF4}" type="CELLRANGE">
+                    <a:fld id="{00241673-CF02-4BEC-85C3-D4657A173CD6}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1752,7 +1749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CEB28D6-F36D-4356-90F7-9C11BF8BB021}" type="CELLRANGE">
+                    <a:fld id="{5B668927-0153-4D80-A398-D76F2E00DB58}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1786,7 +1783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ED9C8E1-07B6-4218-923C-8F6DD816172A}" type="CELLRANGE">
+                    <a:fld id="{1F497C90-BFCB-47C7-A8C9-E06F25A56524}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1820,7 +1817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{398E75BB-5889-489F-8DEC-AFB02450FAC3}" type="CELLRANGE">
+                    <a:fld id="{3A8E9428-ABEF-49AA-866E-1D03C21B123D}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1854,7 +1851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59ACE9C7-BEA6-458F-968C-AAA595553A90}" type="CELLRANGE">
+                    <a:fld id="{71B4CFF9-D266-4506-BB8F-BEC828EC7117}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1888,7 +1885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75F52580-EB60-49ED-B1E8-8DF31BB573F9}" type="CELLRANGE">
+                    <a:fld id="{D2BACF7C-B94F-47DD-80E8-C43237E9FAE3}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1922,7 +1919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D46A55DF-FB5C-4420-8EDC-D473C1907CC6}" type="CELLRANGE">
+                    <a:fld id="{6457D793-6E87-4C88-AE68-36A64E2A423B}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1956,7 +1953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D5656F6-E3DB-4659-AE99-DBFDB2F86A45}" type="CELLRANGE">
+                    <a:fld id="{BEF5D028-7169-43A0-B95F-8E7CCACA5A46}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1990,7 +1987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E6EFFAA-D742-4946-80F0-1A990A350968}" type="CELLRANGE">
+                    <a:fld id="{8D81A419-5A8D-43E1-AD0A-486B5262E7CA}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2024,7 +2021,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15FB13CE-DD63-42B8-B528-3FDB2B9F6FDF}" type="CELLRANGE">
+                    <a:fld id="{99F516EB-4D62-4BB2-96F2-7E2616D69CAA}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2058,7 +2055,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27666DB1-569C-4F2B-862F-815795A03E81}" type="CELLRANGE">
+                    <a:fld id="{E9460853-C664-4831-ACF9-53DCA4554520}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2092,7 +2089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB977E01-BF39-471D-B5ED-7A20D612D286}" type="CELLRANGE">
+                    <a:fld id="{411D2523-7869-4104-82AE-B19446A716DC}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2126,7 +2123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{245F7D05-C48E-4338-A474-858440244293}" type="CELLRANGE">
+                    <a:fld id="{94B118F4-F76C-4F6E-8642-7DE8DD214BF2}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2160,7 +2157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD2DB2AB-9285-4BA2-97CB-051F1D729F4D}" type="CELLRANGE">
+                    <a:fld id="{21B94314-4CAD-4846-9180-741ADCA62234}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2194,7 +2191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED86ADD0-51D3-4E18-99D1-861F1CD39AFD}" type="CELLRANGE">
+                    <a:fld id="{188E1D4F-B97C-48A2-9B23-A571F1403C10}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2228,7 +2225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{931FB98B-0540-4B6B-8EDA-72683CEC5408}" type="CELLRANGE">
+                    <a:fld id="{65423988-8445-4DE0-9771-F8CC57412F53}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2262,7 +2259,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2583F514-57E4-496D-A945-24C96F22E22D}" type="CELLRANGE">
+                    <a:fld id="{DF051D04-C0EB-43F9-9088-64A450137124}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2296,7 +2293,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56E71F4D-605F-4E88-B92C-BB76136452BF}" type="CELLRANGE">
+                    <a:fld id="{ACD4F83F-F633-453F-AE3E-4C8C77C19B4B}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2330,7 +2327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{007E4CC4-AC0E-4796-80E0-CE344422A2CF}" type="CELLRANGE">
+                    <a:fld id="{04412882-87AB-4EC6-925E-CB4FA7A01C1C}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2364,7 +2361,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6385402D-D420-45A6-B5EC-46D4CA4C8050}" type="CELLRANGE">
+                    <a:fld id="{287C195C-DB01-4E40-B37D-82C87932A529}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2398,7 +2395,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C242D57-95ED-4CF4-BD68-6FBDD8D12365}" type="CELLRANGE">
+                    <a:fld id="{84B70749-163D-4469-8878-BBB6539116A5}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3304,7 +3301,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29DA302C-6006-435E-88AD-50790A66A972}" type="CELLRANGE">
+                    <a:fld id="{0C73A6BF-694A-48CA-920A-90F0A0718239}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3337,7 +3334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AB4B6A4-CC1A-4A79-BEC8-B13E68588831}" type="CELLRANGE">
+                    <a:fld id="{8504C208-4C95-4E48-AD06-3302BAFBD3DF}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3371,7 +3368,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD9BDA3E-1183-40DF-9703-82D52CC8B277}" type="CELLRANGE">
+                    <a:fld id="{A1ED206F-235A-49DD-A523-1F7245F1BF87}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3405,7 +3402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8190353D-F681-469A-BB46-2C14AAF9AB80}" type="CELLRANGE">
+                    <a:fld id="{C19DB21B-1096-4EB6-89FE-58EC584657CC}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3439,7 +3436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA093B48-A810-41F2-88FA-07432B9BE322}" type="CELLRANGE">
+                    <a:fld id="{D9C31681-AC99-473E-B8E6-1CF6F995ECA7}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3473,7 +3470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C15857B-8B25-4103-90C8-F0F783F3C8B4}" type="CELLRANGE">
+                    <a:fld id="{00F8A769-22CB-4473-869A-27730F4D413D}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3507,7 +3504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{323DCC75-9F99-48D1-9F96-18AD2F0EB27E}" type="CELLRANGE">
+                    <a:fld id="{0DF3EFCE-D70C-4F5D-B06A-5A6029E6A427}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3541,7 +3538,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8CFA4009-7179-4DB3-ABDA-4427D7488D7A}" type="CELLRANGE">
+                    <a:fld id="{2D880178-0611-4BD0-AFC7-A6F60F6B5933}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3575,7 +3572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2921CC03-1145-48A1-AB5F-19008691207D}" type="CELLRANGE">
+                    <a:fld id="{977385F5-C332-49E7-997D-17027A90FE78}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3609,7 +3606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE61A13D-449E-4B39-8383-328E6034D539}" type="CELLRANGE">
+                    <a:fld id="{37AEA08F-CBD0-48E7-9DA2-7B8515EE2CC3}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3643,7 +3640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D531DAF3-2508-4E47-A990-144ACBBC0C86}" type="CELLRANGE">
+                    <a:fld id="{68AD58F1-3DF8-43C5-83D3-8BD31EE78303}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3677,7 +3674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D281CB2A-52C9-419A-8CB1-C7ABB91A83DB}" type="CELLRANGE">
+                    <a:fld id="{CC9D6BCD-26B7-461C-93CA-95E52FD9D6E9}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3711,7 +3708,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C0E0A7B-317A-4489-9D1B-A94F74D304C1}" type="CELLRANGE">
+                    <a:fld id="{0419E79A-D9E0-4CCF-A592-93EAECC25950}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3745,7 +3742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E9D6517-160D-4FBF-B338-36BC66D0C82F}" type="CELLRANGE">
+                    <a:fld id="{9D32D242-D85E-463F-BA6F-0EC29E592DD5}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3779,7 +3776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02D60AED-9C6D-4788-9A33-48552F6BD2A4}" type="CELLRANGE">
+                    <a:fld id="{2E9E4708-2AD8-43C9-B3A0-CDF226F272A7}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3813,7 +3810,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C92E084-10DB-454E-B93C-44F2703993E2}" type="CELLRANGE">
+                    <a:fld id="{EABF47FF-8E7A-43F9-BF5E-D90B8057FC34}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3847,7 +3844,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43A647C2-A89A-42B1-85A5-CBC2F165AE85}" type="CELLRANGE">
+                    <a:fld id="{5FFAB243-17EC-4778-BEFB-8EEE257DEA7E}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3881,7 +3878,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{706160F1-BF25-4AF0-A4C4-46829F4B18D7}" type="CELLRANGE">
+                    <a:fld id="{72035D3D-490F-477A-8CBD-DDF1BABA0DF9}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3915,7 +3912,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FB165A2-6135-46C2-883E-3413BCECBFCF}" type="CELLRANGE">
+                    <a:fld id="{D21A70DC-AAC3-473C-8586-AF65D47DCBEE}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3949,7 +3946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95D10F79-7D5C-4EA1-9B66-CBB911DF74EC}" type="CELLRANGE">
+                    <a:fld id="{D00FD96D-9E36-4204-B462-6B9AFC1E0DDE}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3983,7 +3980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{187BDCCF-C11A-4C6E-A822-D1E0C8CCA1D2}" type="CELLRANGE">
+                    <a:fld id="{12BE6668-97D6-4147-BA2A-30CDB181D544}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4017,7 +4014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0BC7723-3E6B-4D76-8F2F-14193DA7B295}" type="CELLRANGE">
+                    <a:fld id="{05AFD421-ADD4-489A-A69F-E0EC5EAA483B}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4051,7 +4048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C21F5DB-9DD6-4EF3-A9F3-5AA0F6002C10}" type="CELLRANGE">
+                    <a:fld id="{CB0CF633-C5DB-4AE0-A297-2DD4BEA1BC6D}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8194,7 +8191,7 @@
   <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8208,12 +8205,12 @@
   <sheetData>
     <row r="1" spans="2:3" s="2" customFormat="1">
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="2:3" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:3" s="2" customFormat="1">
@@ -8276,33 +8273,33 @@
     </row>
     <row r="24" spans="2:4" ht="20.25" thickBot="1">
       <c r="B24" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="74" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="74"/>
     </row>
@@ -8312,12 +8309,12 @@
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="2:10" s="2" customFormat="1">
@@ -8392,7 +8389,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -10777,7 +10774,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="25" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -10804,20 +10801,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="52.5" customHeight="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
@@ -10852,11 +10849,11 @@
       <c r="V2" s="29"/>
     </row>
     <row r="3" spans="1:25" ht="15" customHeight="1">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
@@ -10871,10 +10868,10 @@
       <c r="A4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="77"/>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
@@ -10891,10 +10888,10 @@
       <c r="A5" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="85"/>
+      <c r="C5" s="77"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
@@ -10911,10 +10908,10 @@
       <c r="A6" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="85"/>
+      <c r="C6" s="77"/>
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
@@ -10931,10 +10928,10 @@
       <c r="A7" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="85"/>
+      <c r="C7" s="77"/>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -10951,10 +10948,10 @@
       <c r="A8" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="77"/>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
@@ -10972,11 +10969,11 @@
       <c r="D9" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="86" t="str">
+      <c r="E9" s="88" t="str">
         <f>_xlfn.CONCAT(B5," vs. ",B4)</f>
         <v>Cell Internal Resitance (Ω) vs. Cell Nominal Capacity (Ah)</v>
       </c>
-      <c r="F9" s="86"/>
+      <c r="F9" s="88"/>
       <c r="G9" s="29"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
@@ -10994,11 +10991,11 @@
       <c r="D10" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="87" t="str">
+      <c r="E10" s="89" t="str">
         <f>_xlfn.CONCAT(B8)</f>
         <v>Cell Max Charge Current (A)</v>
       </c>
-      <c r="F10" s="87"/>
+      <c r="F10" s="89"/>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
@@ -11031,11 +11028,9 @@
       <c r="V11" s="29"/>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1">
-      <c r="A12" s="88" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -11326,39 +11321,39 @@
       <c r="Y26" s="29"/>
     </row>
     <row r="27" spans="1:25" ht="15">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="92"/>
+      <c r="C27" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="90"/>
-      <c r="C27" s="91" t="s">
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="80" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="81"/>
+      <c r="I27" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="83"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="78"/>
-      <c r="I27" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="80"/>
-      <c r="K27" s="81"/>
-      <c r="L27" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="M27" s="83"/>
-      <c r="N27" s="83"/>
-      <c r="O27" s="83"/>
-      <c r="P27" s="84"/>
+      <c r="M27" s="86"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="86"/>
+      <c r="P27" s="87"/>
     </row>
     <row r="28" spans="1:25" ht="15">
       <c r="A28" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="35" t="s">
         <v>73</v>
@@ -11370,7 +11365,7 @@
         <v>67</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G28" s="39" t="s">
         <v>69</v>
@@ -11379,28 +11374,28 @@
         <v>71</v>
       </c>
       <c r="I28" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="J28" s="42" t="s">
+      <c r="K28" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="K28" s="43" t="s">
+      <c r="L28" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="L28" s="44" t="s">
+      <c r="M28" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="M28" s="44" t="s">
+      <c r="N28" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N28" s="44" t="s">
+      <c r="O28" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="O28" s="44" t="s">
+      <c r="P28" s="44" t="s">
         <v>88</v>
-      </c>
-      <c r="P28" s="44" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -13269,12 +13264,6 @@
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="15">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="L27:P27"/>
@@ -13284,6 +13273,12 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:F27"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5 B8" xr:uid="{A7852E70-5BEE-4D66-A649-520BB2C90F33}">
@@ -13293,14 +13288,11 @@
       <formula1>$G$28:$H$28</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="A12:C12" r:id="rId1" location="SimpleBatteryCharging" display="Open Model In Impact" xr:uid="{5F3A9745-3CBE-4770-9FCD-7CDB0E938A45}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="90" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: correct impact url in experiment sheet
</commit_message>
<xml_diff>
--- a/ExcelSheets/SimpleBatteryCharging.xlsx
+++ b/ExcelSheets/SimpleBatteryCharging.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B803D6B9-3342-4572-B981-BB2D78C7FB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA71C13-4B4C-45DB-AAC6-D24FFF941F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -389,9 +389,6 @@
     <t>dynamic</t>
   </si>
   <si>
-    <t>https://jhmi-staging.modelon.com</t>
-  </si>
-  <si>
     <t>dynamic_diagnostics</t>
   </si>
   <si>
@@ -615,6 +612,9 @@
   </si>
   <si>
     <t>3. First time you open the sheet you will need to use the "Run baseline" button to initialize the experiment sheet.</t>
+  </si>
+  <si>
+    <t>https://impact.modelon.cloud</t>
   </si>
 </sst>
 </file>
@@ -1431,13 +1431,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1462,6 +1455,7 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="14" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1481,6 +1475,12 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1982,7 +1982,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BEC11D1-0DDB-4134-AE7B-8778FB885FE5}" type="CELLRANGE">
+                    <a:fld id="{F13F5ACC-2463-4F75-86E4-403C78CE624F}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2016,7 +2016,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCA8AC75-FCF5-4DEF-993D-70063A343B39}" type="CELLRANGE">
+                    <a:fld id="{56E41C7C-DEAD-46C7-A280-933E01B33944}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2050,7 +2050,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43598C74-3989-4D51-B0F5-97D6B93F459E}" type="CELLRANGE">
+                    <a:fld id="{D03152EB-BFCF-49B6-978C-515F1DCCAC47}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2084,7 +2084,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58329F94-9B6B-448E-A191-F7B5A1D05D16}" type="CELLRANGE">
+                    <a:fld id="{8807AA43-4A93-47D7-81E0-F8EFA7600F29}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2118,7 +2118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{556C45A9-5B48-4EA4-9CBD-AEA21DB2C9D8}" type="CELLRANGE">
+                    <a:fld id="{9D83D1F4-A8BF-4ABB-88BC-EFF6C9470678}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2152,7 +2152,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81B8E6F0-15C0-430F-A09A-516FD9EB0962}" type="CELLRANGE">
+                    <a:fld id="{29233E69-636D-4E78-AB52-C61EDF1F28AD}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2186,7 +2186,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14EEE173-9593-4CCD-9081-DC8FB6B67469}" type="CELLRANGE">
+                    <a:fld id="{E03B68D9-F020-4D9A-8F06-2F87F1D5DF7A}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2220,7 +2220,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{620714F7-1662-4378-B46E-88C67D6FB966}" type="CELLRANGE">
+                    <a:fld id="{1C6FADE8-1BC1-4150-880A-95D602496056}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2254,7 +2254,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE512BCB-0EDF-42F9-A694-981935E55157}" type="CELLRANGE">
+                    <a:fld id="{00F689CA-34E1-4342-AD72-78BFD085556E}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2288,7 +2288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13D3C4EA-C29A-4C51-A697-C37804628559}" type="CELLRANGE">
+                    <a:fld id="{E13C2941-B631-4AEE-B0F3-4B6009B5B030}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2322,7 +2322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{443184B2-AEF1-44AB-890D-F906F98F89F7}" type="CELLRANGE">
+                    <a:fld id="{598F3157-BC1D-4B4A-B3A4-93E05AE1014E}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2356,7 +2356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E22C9A30-34A6-456C-A583-DD5D1F1D913A}" type="CELLRANGE">
+                    <a:fld id="{19965CDF-8459-4138-827E-FA780212EAC7}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2390,7 +2390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5958B628-9499-4F35-BB01-7A1EF51C1AF8}" type="CELLRANGE">
+                    <a:fld id="{C6073AE2-A5CF-4E32-B636-41FFE0E90844}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2424,7 +2424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{479D5FD5-E445-4F01-BD92-7A2EE7445628}" type="CELLRANGE">
+                    <a:fld id="{92EDBE45-7C07-433E-806B-C853DABFAE38}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2458,7 +2458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B11AF68B-45E8-43F0-B799-7F6F5F8446DE}" type="CELLRANGE">
+                    <a:fld id="{AC0DFB7A-C4D9-4527-80C8-EA14A0F448C7}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2492,7 +2492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD90E567-3E39-4BF8-A87D-A2E781A3D050}" type="CELLRANGE">
+                    <a:fld id="{401D2E78-21E8-4F8B-8A8C-F6F942A3608B}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2526,7 +2526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DE49F9C-64FF-4DD5-8E38-5734A7CEADA1}" type="CELLRANGE">
+                    <a:fld id="{61BE5A34-9377-49D6-BC27-1AD81B3EDEB7}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2560,7 +2560,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85917021-79BB-46C1-8FCE-C0FFD17F36A6}" type="CELLRANGE">
+                    <a:fld id="{FA9FDECD-4CB2-412B-9E35-A5CF74625D43}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2594,7 +2594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F5F5C76-1B6B-4FD7-BC30-A4BCE46BA411}" type="CELLRANGE">
+                    <a:fld id="{5D6941A3-470F-457C-8018-AEAF05146AE8}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2628,7 +2628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCC59C1A-8F6B-4932-B042-2AF95A68DD18}" type="CELLRANGE">
+                    <a:fld id="{31A04C73-7111-4423-81BD-72D0A148224B}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2662,7 +2662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23C539FE-BAEE-483A-BE48-272DED0183D7}" type="CELLRANGE">
+                    <a:fld id="{9A8C416E-0A4F-47E9-9FD0-F3CBE29878F9}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2696,7 +2696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E634EA8-415E-4986-8571-C6C778F2DAFB}" type="CELLRANGE">
+                    <a:fld id="{4EA9A11F-8F3B-42A0-93BB-2A6BAF336211}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3663,7 +3663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91FDF5C3-901A-4DB7-9A07-38C0BA0F322C}" type="CELLRANGE">
+                    <a:fld id="{92B82436-38B3-40D5-9AA3-B0A2A71B67C8}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3837,7 +3837,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A295DE88-FFD0-488A-8FB3-AAB58B290EFE}" type="CELLRANGE">
+                    <a:fld id="{8B5F07C9-F975-4A42-BBBF-3CB946FDFFF3}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4011,7 +4011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8F26EAF-62C2-4FF9-8F30-C3EBCA990D69}" type="CELLRANGE">
+                    <a:fld id="{A92312FD-FDD7-4259-823F-AB03EF81BD8C}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4101,7 +4101,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CEA1B95-A54D-413B-9E76-241E8CB3A1A3}" type="CELLRANGE">
+                    <a:fld id="{F03661CB-E454-496C-9358-C54550C43F80}" type="CELLRANGE">
                       <a:rPr lang="en-SE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8501,7 +8501,7 @@
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D31" s="72"/>
     </row>
@@ -8551,7 +8551,7 @@
   <dimension ref="A1:AI50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -8623,7 +8623,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -8709,7 +8709,7 @@
         <v>103</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:35" collapsed="1">
@@ -8724,7 +8724,7 @@
     </row>
     <row r="16" spans="1:35" ht="17.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="74" t="b">
         <v>0</v>
@@ -8732,7 +8732,7 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="74">
         <v>500</v>
@@ -8750,7 +8750,7 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E20" s="74">
         <v>9.9999999999999995E-7</v>
@@ -8768,15 +8768,15 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="17.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E24" s="74" t="b">
         <v>0</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E25" s="74" t="b">
         <v>0</v>
@@ -9196,7 +9196,7 @@
         <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="75">
@@ -9298,7 +9298,7 @@
         <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D34" s="13"/>
       <c r="E34" s="75">
@@ -9400,7 +9400,7 @@
         <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="75">
@@ -9746,7 +9746,7 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D41" s="73" t="b">
         <v>0</v>
@@ -9850,7 +9850,7 @@
         <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D42" s="74" t="b">
         <v>0</v>
@@ -9959,94 +9959,94 @@
         <v>16</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="V45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AB45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AC45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AD45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AG45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AH45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1">
@@ -10089,94 +10089,94 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G47" t="s">
         <v>154</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>155</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>156</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>157</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>158</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>159</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
+        <v>154</v>
+      </c>
+      <c r="N47" t="s">
         <v>160</v>
       </c>
-      <c r="M47" t="s">
-        <v>155</v>
-      </c>
-      <c r="N47" t="s">
+      <c r="O47" t="s">
         <v>161</v>
       </c>
-      <c r="O47" t="s">
+      <c r="P47" t="s">
         <v>162</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>163</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="R47" t="s">
         <v>164</v>
       </c>
-      <c r="R47" t="s">
+      <c r="S47" t="s">
         <v>165</v>
       </c>
-      <c r="S47" t="s">
+      <c r="T47" t="s">
         <v>166</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
+        <v>161</v>
+      </c>
+      <c r="V47" t="s">
         <v>167</v>
       </c>
-      <c r="U47" t="s">
-        <v>162</v>
-      </c>
-      <c r="V47" t="s">
+      <c r="W47" t="s">
         <v>168</v>
       </c>
-      <c r="W47" t="s">
+      <c r="X47" t="s">
         <v>169</v>
       </c>
-      <c r="X47" t="s">
+      <c r="Y47" t="s">
         <v>170</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>171</v>
       </c>
-      <c r="Z47" t="s">
+      <c r="AA47" t="s">
         <v>172</v>
       </c>
-      <c r="AA47" t="s">
+      <c r="AB47" t="s">
         <v>173</v>
       </c>
-      <c r="AB47" t="s">
+      <c r="AC47" t="s">
         <v>174</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="AD47" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE47" t="s">
         <v>175</v>
       </c>
-      <c r="AD47" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE47" t="s">
+      <c r="AF47" t="s">
         <v>176</v>
       </c>
-      <c r="AF47" t="s">
+      <c r="AG47" t="s">
         <v>177</v>
       </c>
-      <c r="AG47" t="s">
+      <c r="AH47" t="s">
         <v>178</v>
       </c>
-      <c r="AH47" t="s">
+      <c r="AI47" t="s">
         <v>179</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:35">
@@ -10184,94 +10184,94 @@
         <v>19</v>
       </c>
       <c r="F48" t="s">
+        <v>180</v>
+      </c>
+      <c r="G48" t="s">
+        <v>180</v>
+      </c>
+      <c r="H48" t="s">
+        <v>180</v>
+      </c>
+      <c r="I48" t="s">
+        <v>180</v>
+      </c>
+      <c r="J48" t="s">
+        <v>180</v>
+      </c>
+      <c r="K48" t="s">
+        <v>180</v>
+      </c>
+      <c r="L48" t="s">
+        <v>180</v>
+      </c>
+      <c r="M48" t="s">
+        <v>180</v>
+      </c>
+      <c r="N48" t="s">
         <v>181</v>
       </c>
-      <c r="G48" t="s">
+      <c r="O48" t="s">
         <v>181</v>
       </c>
-      <c r="H48" t="s">
+      <c r="P48" t="s">
         <v>181</v>
       </c>
-      <c r="I48" t="s">
+      <c r="Q48" t="s">
         <v>181</v>
       </c>
-      <c r="J48" t="s">
+      <c r="R48" t="s">
         <v>181</v>
       </c>
-      <c r="K48" t="s">
+      <c r="S48" t="s">
         <v>181</v>
       </c>
-      <c r="L48" t="s">
+      <c r="T48" t="s">
         <v>181</v>
       </c>
-      <c r="M48" t="s">
+      <c r="U48" t="s">
         <v>181</v>
       </c>
-      <c r="N48" t="s">
-        <v>182</v>
-      </c>
-      <c r="O48" t="s">
-        <v>182</v>
-      </c>
-      <c r="P48" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>182</v>
-      </c>
-      <c r="R48" t="s">
-        <v>182</v>
-      </c>
-      <c r="S48" t="s">
-        <v>182</v>
-      </c>
-      <c r="T48" t="s">
-        <v>182</v>
-      </c>
-      <c r="U48" t="s">
-        <v>182</v>
-      </c>
       <c r="V48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="W48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Y48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AB48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AC48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AE48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AF48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AG48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AH48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AI48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="2:35">
@@ -10279,7 +10279,7 @@
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G49"/>
       <c r="H49"/>
@@ -10316,94 +10316,94 @@
         <v>21</v>
       </c>
       <c r="F50" t="s">
+        <v>121</v>
+      </c>
+      <c r="G50" t="s">
         <v>122</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>123</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>124</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>125</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>126</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>127</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>128</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>129</v>
       </c>
-      <c r="N50" t="s">
+      <c r="O50" t="s">
         <v>130</v>
       </c>
-      <c r="O50" t="s">
+      <c r="P50" t="s">
         <v>131</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>132</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>133</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>134</v>
       </c>
-      <c r="S50" t="s">
+      <c r="T50" t="s">
         <v>135</v>
       </c>
-      <c r="T50" t="s">
+      <c r="U50" t="s">
         <v>136</v>
       </c>
-      <c r="U50" t="s">
+      <c r="V50" t="s">
         <v>137</v>
       </c>
-      <c r="V50" t="s">
+      <c r="W50" t="s">
         <v>138</v>
       </c>
-      <c r="W50" t="s">
+      <c r="X50" t="s">
         <v>139</v>
       </c>
-      <c r="X50" t="s">
+      <c r="Y50" t="s">
         <v>140</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>141</v>
       </c>
-      <c r="Z50" t="s">
+      <c r="AA50" t="s">
         <v>142</v>
       </c>
-      <c r="AA50" t="s">
+      <c r="AB50" t="s">
         <v>143</v>
       </c>
-      <c r="AB50" t="s">
+      <c r="AC50" t="s">
         <v>144</v>
       </c>
-      <c r="AC50" t="s">
+      <c r="AD50" t="s">
         <v>145</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AE50" t="s">
         <v>146</v>
       </c>
-      <c r="AE50" t="s">
+      <c r="AF50" t="s">
         <v>147</v>
       </c>
-      <c r="AF50" t="s">
+      <c r="AG50" t="s">
         <v>148</v>
       </c>
-      <c r="AG50" t="s">
+      <c r="AH50" t="s">
         <v>149</v>
       </c>
-      <c r="AH50" t="s">
+      <c r="AI50" t="s">
         <v>150</v>
-      </c>
-      <c r="AI50" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -11677,20 +11677,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="52.5" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
       <c r="O1" s="22"/>
@@ -11725,11 +11725,11 @@
       <c r="V2" s="25"/>
     </row>
     <row r="3" spans="1:25" ht="15" customHeight="1">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -11744,10 +11744,10 @@
       <c r="A4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="78"/>
+      <c r="C4" s="86"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -11764,10 +11764,10 @@
       <c r="A5" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="78"/>
+      <c r="C5" s="86"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -11784,10 +11784,10 @@
       <c r="A6" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="78"/>
+      <c r="C6" s="86"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -11804,10 +11804,10 @@
       <c r="A7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="78"/>
+      <c r="C7" s="86"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -11824,10 +11824,10 @@
       <c r="A8" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="78"/>
+      <c r="C8" s="86"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -11845,11 +11845,11 @@
       <c r="D9" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="89" t="str">
+      <c r="E9" s="87" t="str">
         <f>_xlfn.CONCAT(B5," vs. ",B4)</f>
         <v>Cell Internal Resitance (Ω) vs. Cell Nominal Capacity (Ah)</v>
       </c>
-      <c r="F9" s="89"/>
+      <c r="F9" s="87"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -11867,11 +11867,11 @@
       <c r="D10" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="90" t="str">
+      <c r="E10" s="88" t="str">
         <f>_xlfn.CONCAT(B8)</f>
         <v>Cell Max Charge Current (A)</v>
       </c>
-      <c r="F10" s="90"/>
+      <c r="F10" s="88"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -11904,9 +11904,9 @@
       <c r="V11" s="25"/>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1">
-      <c r="A12" s="91"/>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
@@ -12197,32 +12197,32 @@
       <c r="Y26" s="25"/>
     </row>
     <row r="27" spans="1:25" ht="15">
-      <c r="A27" s="92" t="s">
+      <c r="A27" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="94" t="s">
+      <c r="B27" s="91"/>
+      <c r="C27" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="81" t="s">
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="82"/>
-      <c r="I27" s="83" t="s">
+      <c r="H27" s="79"/>
+      <c r="I27" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="J27" s="84"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="86" t="s">
+      <c r="J27" s="81"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="87"/>
-      <c r="N27" s="87"/>
-      <c r="O27" s="87"/>
-      <c r="P27" s="88"/>
+      <c r="M27" s="84"/>
+      <c r="N27" s="84"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="85"/>
     </row>
     <row r="28" spans="1:25" ht="15">
       <c r="A28" s="29" t="s">
@@ -14140,6 +14140,12 @@
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="15">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="L27:P27"/>
@@ -14149,12 +14155,6 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:F27"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5 B8" xr:uid="{A7852E70-5BEE-4D66-A649-520BB2C90F33}">

</xml_diff>